<commit_message>
sharing, settings almost finished
</commit_message>
<xml_diff>
--- a/Features Checklist.xlsx
+++ b/Features Checklist.xlsx
@@ -490,7 +490,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -513,8 +513,8 @@
       <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
@@ -562,11 +562,15 @@
       <c r="A9" t="s">
         <v>7</v>
       </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
@@ -577,6 +581,8 @@
       <c r="A12" t="s">
         <v>13</v>
       </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>